<commit_message>
temp: try to handle stirrup graph
</commit_message>
<xml_diff>
--- a/assets/example2/example2.xlsx
+++ b/assets/example2/example2.xlsx
@@ -737,7 +737,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-20 17:21:58 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-20 17:38:05 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -1050,7 +1050,7 @@
     <row r="14">
       <c r="A14" s="4" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-20 17:21:58 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-20 17:38:05 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-20 17:21:58 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-20 17:38:05 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: handle tie pattern
</commit_message>
<xml_diff>
--- a/assets/example2/example2.xlsx
+++ b/assets/example2/example2.xlsx
@@ -12,8 +12,8 @@
     <sheet name="特殊鋼筋" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'繫筋家族'!$A$2:$H$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'繫筋家族'!$A$1:$H$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'繫筋家族'!$A$2:$H$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'繫筋家族'!$A$1:$H$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'箍筋家族'!$A$2:$H$14</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'箍筋家族'!$A$1:$H$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'特殊鋼筋'!$A$2:$H$5</definedName>
@@ -51,10 +51,6 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
       <b val="1"/>
       <sz val="12"/>
     </font>
@@ -66,6 +62,10 @@
     <font>
       <name val="Calibri"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="4">
@@ -123,21 +123,21 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -216,6 +216,161 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1143000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1143000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>5</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1143000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>6</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1143000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1143000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>8</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1143000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -659,7 +814,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -734,18 +889,248 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>生成時間：2025-06-20 17:38:05 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+    <row r="4" ht="90" customHeight="1">
+      <c r="A4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>#4</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr"/>
+      <c r="D4" s="4" t="n">
+        <v>102</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>101</v>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>梁繫</t>
+        </is>
+      </c>
+      <c r="H4" s="4" t="inlineStr">
+        <is>
+          <t>梁繫#4-101.5x20</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="90" customHeight="1">
+      <c r="A5" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>#3</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>561</v>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>梁繫</t>
+        </is>
+      </c>
+      <c r="H5" s="4" t="inlineStr">
+        <is>
+          <t>梁繫#3-1000x20</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="90" customHeight="1">
+      <c r="A6" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>#5</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr"/>
+      <c r="D6" s="4" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>4656</v>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>柱繫</t>
+        </is>
+      </c>
+      <c r="H6" s="4" t="inlineStr">
+        <is>
+          <t>柱繫#5-3000x20</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="90" customHeight="1">
+      <c r="A7" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>#5</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr"/>
+      <c r="D7" s="4" t="n">
+        <v>556</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>862</v>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>柱繫</t>
+        </is>
+      </c>
+      <c r="H7" s="4" t="inlineStr">
+        <is>
+          <t>柱繫#5-555.5x20</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="90" customHeight="1">
+      <c r="A8" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>#3</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr"/>
+      <c r="D8" s="4" t="n">
+        <v>51</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="G8" s="4" t="inlineStr">
+        <is>
+          <t>牆繫</t>
+        </is>
+      </c>
+      <c r="H8" s="4" t="inlineStr">
+        <is>
+          <t>牆繫#3-51x20</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="90" customHeight="1">
+      <c r="A9" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>#4</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="inlineStr"/>
+      <c r="D9" s="4" t="n">
+        <v>62</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>62</v>
+      </c>
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t>牆繫</t>
+        </is>
+      </c>
+      <c r="H9" s="4" t="inlineStr">
+        <is>
+          <t>牆繫#4-62.5x20</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>統計摘要</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>總數量</t>
+        </is>
+      </c>
+      <c r="B12" s="8" t="inlineStr">
+        <is>
+          <t>120 支</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr">
+        <is>
+          <t>總重量</t>
+        </is>
+      </c>
+      <c r="D12" s="8" t="inlineStr">
+        <is>
+          <t>6271.00 kg</t>
+        </is>
+      </c>
+      <c r="E12" s="7" t="inlineStr">
+        <is>
+          <t>總長度</t>
+        </is>
+      </c>
+      <c r="F12" s="8" t="inlineStr">
+        <is>
+          <t>95420 cm</t>
+        </is>
+      </c>
+      <c r="G12" s="7" t="inlineStr">
+        <is>
+          <t>鋼筋類型</t>
+        </is>
+      </c>
+      <c r="H12" s="8" t="inlineStr">
+        <is>
+          <t>3 種</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="9" t="inlineStr">
+        <is>
+          <t>生成時間：2025-06-23 13:28:21 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H5"/>
-  <mergeCells count="3">
+  <autoFilter ref="A2:H14"/>
+  <mergeCells count="4">
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A14:H14"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A5:H5"/>
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
@@ -758,6 +1143,7 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -843,214 +1229,214 @@
       </c>
     </row>
     <row r="4" ht="90" customHeight="1">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B4" s="4" t="inlineStr">
         <is>
           <t>#5</t>
         </is>
       </c>
-      <c r="C4" s="6" t="inlineStr"/>
-      <c r="D4" s="5" t="n">
+      <c r="C4" s="5" t="inlineStr"/>
+      <c r="D4" s="4" t="n">
         <v>125</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="4" t="n">
         <v>194</v>
       </c>
-      <c r="G4" s="5" t="inlineStr"/>
-      <c r="H4" s="5" t="inlineStr">
+      <c r="G4" s="4" t="inlineStr"/>
+      <c r="H4" s="4" t="inlineStr">
         <is>
           <t>地箍#5(50x75)=20</t>
         </is>
       </c>
     </row>
     <row r="5" ht="90" customHeight="1">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>#4</t>
         </is>
       </c>
-      <c r="C5" s="6" t="inlineStr"/>
-      <c r="D5" s="5" t="n">
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="4" t="n">
         <v>125</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="4" t="n">
         <v>124</v>
       </c>
-      <c r="G5" s="5" t="inlineStr"/>
-      <c r="H5" s="5" t="inlineStr">
+      <c r="G5" s="4" t="inlineStr"/>
+      <c r="H5" s="4" t="inlineStr">
         <is>
           <t>L箍#4(50+75)=20</t>
         </is>
       </c>
     </row>
     <row r="6" ht="90" customHeight="1">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B6" s="4" t="inlineStr">
         <is>
           <t>#5</t>
         </is>
       </c>
-      <c r="C6" s="6" t="inlineStr"/>
-      <c r="D6" s="5" t="n">
+      <c r="C6" s="5" t="inlineStr"/>
+      <c r="D6" s="4" t="n">
         <v>125</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="4" t="n">
         <v>194</v>
       </c>
-      <c r="G6" s="5" t="inlineStr"/>
-      <c r="H6" s="5" t="inlineStr">
+      <c r="G6" s="4" t="inlineStr"/>
+      <c r="H6" s="4" t="inlineStr">
         <is>
           <t>U箍#5(50x75)=20</t>
         </is>
       </c>
     </row>
     <row r="7" ht="90" customHeight="1">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>#4</t>
         </is>
       </c>
-      <c r="C7" s="6" t="inlineStr"/>
-      <c r="D7" s="5" t="n">
+      <c r="C7" s="5" t="inlineStr"/>
+      <c r="D7" s="4" t="n">
         <v>125</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F7" s="5" t="n">
+      <c r="F7" s="4" t="n">
         <v>124</v>
       </c>
-      <c r="G7" s="5" t="inlineStr"/>
-      <c r="H7" s="5" t="inlineStr">
+      <c r="G7" s="4" t="inlineStr"/>
+      <c r="H7" s="4" t="inlineStr">
         <is>
           <t>牆箍#4(50x75)=20</t>
         </is>
       </c>
     </row>
     <row r="8" ht="90" customHeight="1">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="5" t="inlineStr">
+      <c r="B8" s="4" t="inlineStr">
         <is>
           <t>#4</t>
         </is>
       </c>
-      <c r="C8" s="6" t="inlineStr"/>
-      <c r="D8" s="5" t="n">
+      <c r="C8" s="5" t="inlineStr"/>
+      <c r="D8" s="4" t="n">
         <v>125</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="4" t="n">
         <v>124</v>
       </c>
-      <c r="G8" s="5" t="inlineStr"/>
-      <c r="H8" s="5" t="inlineStr">
+      <c r="G8" s="4" t="inlineStr"/>
+      <c r="H8" s="4" t="inlineStr">
         <is>
           <t>柱箍#4(50x75)=20</t>
         </is>
       </c>
     </row>
     <row r="9" ht="90" customHeight="1">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr">
         <is>
           <t>#3</t>
         </is>
       </c>
-      <c r="C9" s="6" t="inlineStr"/>
-      <c r="D9" s="5" t="n">
+      <c r="C9" s="5" t="inlineStr"/>
+      <c r="D9" s="4" t="n">
         <v>125</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F9" s="5" t="n">
+      <c r="F9" s="4" t="n">
         <v>70</v>
       </c>
-      <c r="G9" s="5" t="inlineStr"/>
-      <c r="H9" s="5" t="inlineStr">
+      <c r="G9" s="4" t="inlineStr"/>
+      <c r="H9" s="4" t="inlineStr">
         <is>
           <t>半箍#3(50+75)=20</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="inlineStr">
+      <c r="A11" s="6" t="inlineStr">
         <is>
           <t>統計摘要</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="inlineStr">
+      <c r="A12" s="7" t="inlineStr">
         <is>
           <t>總數量</t>
         </is>
       </c>
-      <c r="B12" s="9" t="inlineStr">
+      <c r="B12" s="8" t="inlineStr">
         <is>
           <t>120 支</t>
         </is>
       </c>
-      <c r="C12" s="8" t="inlineStr">
+      <c r="C12" s="7" t="inlineStr">
         <is>
           <t>總重量</t>
         </is>
       </c>
-      <c r="D12" s="9" t="inlineStr">
+      <c r="D12" s="8" t="inlineStr">
         <is>
           <t>830.00 kg</t>
         </is>
       </c>
-      <c r="E12" s="8" t="inlineStr">
+      <c r="E12" s="7" t="inlineStr">
         <is>
           <t>總長度</t>
         </is>
       </c>
-      <c r="F12" s="9" t="inlineStr">
+      <c r="F12" s="8" t="inlineStr">
         <is>
           <t>15000 cm</t>
         </is>
       </c>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G12" s="7" t="inlineStr">
         <is>
           <t>鋼筋類型</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
+      <c r="H12" s="8" t="inlineStr">
         <is>
           <t>3 種</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>生成時間：2025-06-20 17:38:05 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+      <c r="A14" s="9" t="inlineStr">
+        <is>
+          <t>生成時間：2025-06-23 13:28:21 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -1158,9 +1544,9 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>生成時間：2025-06-20 17:38:05 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+      <c r="A5" s="9" t="inlineStr">
+        <is>
+          <t>生成時間：2025-06-23 13:28:21 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: handle custom type
</commit_message>
<xml_diff>
--- a/assets/example2/example2.xlsx
+++ b/assets/example2/example2.xlsx
@@ -16,8 +16,8 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'繫筋家族'!$A$1:$H$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'箍筋家族'!$A$2:$H$14</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'箍筋家族'!$A$1:$H$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'特殊鋼筋'!$A$2:$H$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'特殊鋼筋'!$A$1:$H$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'特殊鋼筋'!$A$2:$H$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'特殊鋼筋'!$A$1:$H$12</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -525,6 +525,111 @@
 </wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1143000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1143000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>5</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1143000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>6</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3333750" cy="1143000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1121,7 +1226,7 @@
     <row r="14">
       <c r="A14" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-23 13:28:21 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-23 13:48:36 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -1436,7 +1541,7 @@
     <row r="14">
       <c r="A14" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-23 13:28:21 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-23 13:48:36 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
@@ -1468,7 +1573,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -1543,18 +1648,188 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="9" t="inlineStr">
-        <is>
-          <t>生成時間：2025-06-23 13:28:21 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+    <row r="4" ht="90" customHeight="1">
+      <c r="A4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>#5</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr"/>
+      <c r="D4" s="4" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>4656</v>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>安</t>
+        </is>
+      </c>
+      <c r="H4" s="4" t="inlineStr">
+        <is>
+          <t>安#5-3000x20</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="90" customHeight="1">
+      <c r="A5" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>#5</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="4" t="n">
+        <v>85</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>132</v>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>安</t>
+        </is>
+      </c>
+      <c r="H5" s="4" t="inlineStr">
+        <is>
+          <t>安#5-85x20</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="90" customHeight="1">
+      <c r="A6" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>#5</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr"/>
+      <c r="D6" s="4" t="n">
+        <v>1025</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>1591</v>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>安</t>
+        </is>
+      </c>
+      <c r="H6" s="4" t="inlineStr">
+        <is>
+          <t>安#5-25+1000x20</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="90" customHeight="1">
+      <c r="A7" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>#4</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr"/>
+      <c r="D7" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>安</t>
+        </is>
+      </c>
+      <c r="H7" s="4" t="inlineStr">
+        <is>
+          <t>安#4-30+60x20</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>統計摘要</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>總數量</t>
+        </is>
+      </c>
+      <c r="B10" s="8" t="inlineStr">
+        <is>
+          <t>80 支</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr">
+        <is>
+          <t>總重量</t>
+        </is>
+      </c>
+      <c r="D10" s="8" t="inlineStr">
+        <is>
+          <t>6469.00 kg</t>
+        </is>
+      </c>
+      <c r="E10" s="7" t="inlineStr">
+        <is>
+          <t>總長度</t>
+        </is>
+      </c>
+      <c r="F10" s="8" t="inlineStr">
+        <is>
+          <t>84000 cm</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr">
+        <is>
+          <t>鋼筋類型</t>
+        </is>
+      </c>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>2 種</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="9" t="inlineStr">
+        <is>
+          <t>生成時間：2025-06-23 13:48:36 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H5"/>
-  <mergeCells count="3">
+  <autoFilter ref="A2:H12"/>
+  <mergeCells count="4">
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A12:H12"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A5:H5"/>
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
@@ -1567,5 +1842,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add extra column
</commit_message>
<xml_diff>
--- a/assets/example2/example2.xlsx
+++ b/assets/example2/example2.xlsx
@@ -12,12 +12,12 @@
     <sheet name="特殊鋼筋" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'繫筋家族'!$A$2:$H$14</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'繫筋家族'!$A$1:$H$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'箍筋家族'!$A$2:$H$14</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'箍筋家族'!$A$1:$H$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'特殊鋼筋'!$A$2:$H$12</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'特殊鋼筋'!$A$1:$H$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'繫筋家族'!$A$2:$O$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'繫筋家族'!$A$1:$O$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'箍筋家族'!$A$2:$O$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'箍筋家族'!$A$1:$O$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'特殊鋼筋'!$A$2:$O$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'特殊鋼筋'!$A$1:$O$12</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -219,7 +219,7 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>3</row>
       <rowOff>0</rowOff>
@@ -244,7 +244,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>4</row>
       <rowOff>0</rowOff>
@@ -269,7 +269,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>5</row>
       <rowOff>0</rowOff>
@@ -294,7 +294,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>6</row>
       <rowOff>0</rowOff>
@@ -319,7 +319,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>7</row>
       <rowOff>0</rowOff>
@@ -344,7 +344,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>8</row>
       <rowOff>0</rowOff>
@@ -374,7 +374,7 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>3</row>
       <rowOff>0</rowOff>
@@ -399,7 +399,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>4</row>
       <rowOff>0</rowOff>
@@ -424,7 +424,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>5</row>
       <rowOff>0</rowOff>
@@ -449,7 +449,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>6</row>
       <rowOff>0</rowOff>
@@ -474,7 +474,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>7</row>
       <rowOff>0</rowOff>
@@ -499,7 +499,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>8</row>
       <rowOff>0</rowOff>
@@ -529,7 +529,7 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>3</row>
       <rowOff>0</rowOff>
@@ -554,7 +554,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>4</row>
       <rowOff>0</rowOff>
@@ -579,7 +579,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>5</row>
       <rowOff>0</rowOff>
@@ -604,7 +604,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>9</col>
       <colOff>0</colOff>
       <row>6</row>
       <rowOff>0</rowOff>
@@ -919,7 +919,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -929,13 +929,20 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="60" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="45" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="9" max="9"/>
+    <col width="60" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="45" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -965,30 +972,65 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
+          <t>A(cm)</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>B(cm)</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>C(cm)</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>D(cm)</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>E(cm)</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>F(cm)</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>G(cm)</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
           <t>圖示</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="K3" s="3" t="inlineStr">
         <is>
           <t>長度(cm)</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="L3" s="3" t="inlineStr">
         <is>
           <t>數量</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="M3" s="3" t="inlineStr">
         <is>
           <t>重量(kg)</t>
         </is>
       </c>
-      <c r="G3" s="3" t="inlineStr">
+      <c r="N3" s="3" t="inlineStr">
         <is>
           <t>備註</t>
         </is>
       </c>
-      <c r="H3" s="3" t="inlineStr">
+      <c r="O3" s="3" t="inlineStr">
         <is>
           <t>讀取CAD文字</t>
         </is>
@@ -1003,22 +1045,31 @@
           <t>#4</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr"/>
-      <c r="D4" s="4" t="n">
+      <c r="C4" s="4" t="n">
+        <v>101.5</v>
+      </c>
+      <c r="D4" s="4" t="n"/>
+      <c r="E4" s="4" t="n"/>
+      <c r="F4" s="4" t="n"/>
+      <c r="G4" s="4" t="n"/>
+      <c r="H4" s="4" t="n"/>
+      <c r="I4" s="4" t="n"/>
+      <c r="J4" s="5" t="inlineStr"/>
+      <c r="K4" s="4" t="n">
         <v>102</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="L4" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="M4" s="4" t="n">
         <v>101</v>
       </c>
-      <c r="G4" s="4" t="inlineStr">
+      <c r="N4" s="4" t="inlineStr">
         <is>
           <t>梁繫</t>
         </is>
       </c>
-      <c r="H4" s="4" t="inlineStr">
+      <c r="O4" s="4" t="inlineStr">
         <is>
           <t>梁繫#4-101.5x20</t>
         </is>
@@ -1033,22 +1084,31 @@
           <t>#3</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr"/>
-      <c r="D5" s="4" t="n">
+      <c r="C5" s="4" t="n">
         <v>1000</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="D5" s="4" t="n"/>
+      <c r="E5" s="4" t="n"/>
+      <c r="F5" s="4" t="n"/>
+      <c r="G5" s="4" t="n"/>
+      <c r="H5" s="4" t="n"/>
+      <c r="I5" s="4" t="n"/>
+      <c r="J5" s="5" t="inlineStr"/>
+      <c r="K5" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L5" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="M5" s="4" t="n">
         <v>561</v>
       </c>
-      <c r="G5" s="4" t="inlineStr">
+      <c r="N5" s="4" t="inlineStr">
         <is>
           <t>梁繫</t>
         </is>
       </c>
-      <c r="H5" s="4" t="inlineStr">
+      <c r="O5" s="4" t="inlineStr">
         <is>
           <t>梁繫#3-1000x20</t>
         </is>
@@ -1063,22 +1123,31 @@
           <t>#5</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr"/>
-      <c r="D6" s="4" t="n">
+      <c r="C6" s="4" t="n">
         <v>3000</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="D6" s="4" t="n"/>
+      <c r="E6" s="4" t="n"/>
+      <c r="F6" s="4" t="n"/>
+      <c r="G6" s="4" t="n"/>
+      <c r="H6" s="4" t="n"/>
+      <c r="I6" s="4" t="n"/>
+      <c r="J6" s="5" t="inlineStr"/>
+      <c r="K6" s="4" t="n">
+        <v>3000</v>
+      </c>
+      <c r="L6" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="M6" s="4" t="n">
         <v>4656</v>
       </c>
-      <c r="G6" s="4" t="inlineStr">
+      <c r="N6" s="4" t="inlineStr">
         <is>
           <t>柱繫</t>
         </is>
       </c>
-      <c r="H6" s="4" t="inlineStr">
+      <c r="O6" s="4" t="inlineStr">
         <is>
           <t>柱繫#5-3000x20</t>
         </is>
@@ -1093,22 +1162,31 @@
           <t>#5</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr"/>
-      <c r="D7" s="4" t="n">
+      <c r="C7" s="4" t="n">
+        <v>555.5</v>
+      </c>
+      <c r="D7" s="4" t="n"/>
+      <c r="E7" s="4" t="n"/>
+      <c r="F7" s="4" t="n"/>
+      <c r="G7" s="4" t="n"/>
+      <c r="H7" s="4" t="n"/>
+      <c r="I7" s="4" t="n"/>
+      <c r="J7" s="5" t="inlineStr"/>
+      <c r="K7" s="4" t="n">
         <v>556</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="L7" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="M7" s="4" t="n">
         <v>862</v>
       </c>
-      <c r="G7" s="4" t="inlineStr">
+      <c r="N7" s="4" t="inlineStr">
         <is>
           <t>柱繫</t>
         </is>
       </c>
-      <c r="H7" s="4" t="inlineStr">
+      <c r="O7" s="4" t="inlineStr">
         <is>
           <t>柱繫#5-555.5x20</t>
         </is>
@@ -1123,22 +1201,31 @@
           <t>#3</t>
         </is>
       </c>
-      <c r="C8" s="5" t="inlineStr"/>
-      <c r="D8" s="4" t="n">
+      <c r="C8" s="4" t="n">
         <v>51</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="D8" s="4" t="n"/>
+      <c r="E8" s="4" t="n"/>
+      <c r="F8" s="4" t="n"/>
+      <c r="G8" s="4" t="n"/>
+      <c r="H8" s="4" t="n"/>
+      <c r="I8" s="4" t="n"/>
+      <c r="J8" s="5" t="inlineStr"/>
+      <c r="K8" s="4" t="n">
+        <v>51</v>
+      </c>
+      <c r="L8" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F8" s="4" t="n">
+      <c r="M8" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="G8" s="4" t="inlineStr">
+      <c r="N8" s="4" t="inlineStr">
         <is>
           <t>牆繫</t>
         </is>
       </c>
-      <c r="H8" s="4" t="inlineStr">
+      <c r="O8" s="4" t="inlineStr">
         <is>
           <t>牆繫#3-51x20</t>
         </is>
@@ -1153,22 +1240,31 @@
           <t>#4</t>
         </is>
       </c>
-      <c r="C9" s="5" t="inlineStr"/>
-      <c r="D9" s="4" t="n">
+      <c r="C9" s="4" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="D9" s="4" t="n"/>
+      <c r="E9" s="4" t="n"/>
+      <c r="F9" s="4" t="n"/>
+      <c r="G9" s="4" t="n"/>
+      <c r="H9" s="4" t="n"/>
+      <c r="I9" s="4" t="n"/>
+      <c r="J9" s="5" t="inlineStr"/>
+      <c r="K9" s="4" t="n">
         <v>62</v>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="L9" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="M9" s="4" t="n">
         <v>62</v>
       </c>
-      <c r="G9" s="4" t="inlineStr">
+      <c r="N9" s="4" t="inlineStr">
         <is>
           <t>牆繫</t>
         </is>
       </c>
-      <c r="H9" s="4" t="inlineStr">
+      <c r="O9" s="4" t="inlineStr">
         <is>
           <t>牆繫#4-62.5x20</t>
         </is>
@@ -1226,17 +1322,17 @@
     <row r="14">
       <c r="A14" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-23 13:48:36 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-23 14:06:48 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H14"/>
+  <autoFilter ref="A2:O14"/>
   <mergeCells count="4">
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A11:O11"/>
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="A2:O2"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape"/>
@@ -1258,7 +1354,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -1268,13 +1364,20 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="60" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="45" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="9" max="9"/>
+    <col width="60" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="45" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -1304,30 +1407,65 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
+          <t>A(cm)</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>B(cm)</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>C(cm)</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>D(cm)</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>E(cm)</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>F(cm)</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>G(cm)</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
           <t>圖示</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="K3" s="3" t="inlineStr">
         <is>
           <t>長度(cm)</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="L3" s="3" t="inlineStr">
         <is>
           <t>數量</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="M3" s="3" t="inlineStr">
         <is>
           <t>重量(kg)</t>
         </is>
       </c>
-      <c r="G3" s="3" t="inlineStr">
+      <c r="N3" s="3" t="inlineStr">
         <is>
           <t>備註</t>
         </is>
       </c>
-      <c r="H3" s="3" t="inlineStr">
+      <c r="O3" s="3" t="inlineStr">
         <is>
           <t>讀取CAD文字</t>
         </is>
@@ -1342,18 +1480,29 @@
           <t>#5</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr"/>
+      <c r="C4" s="4" t="n">
+        <v>50</v>
+      </c>
       <c r="D4" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="E4" s="4" t="n"/>
+      <c r="F4" s="4" t="n"/>
+      <c r="G4" s="4" t="n"/>
+      <c r="H4" s="4" t="n"/>
+      <c r="I4" s="4" t="n"/>
+      <c r="J4" s="5" t="inlineStr"/>
+      <c r="K4" s="4" t="n">
         <v>125</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="L4" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="M4" s="4" t="n">
         <v>194</v>
       </c>
-      <c r="G4" s="4" t="inlineStr"/>
-      <c r="H4" s="4" t="inlineStr">
+      <c r="N4" s="4" t="inlineStr"/>
+      <c r="O4" s="4" t="inlineStr">
         <is>
           <t>地箍#5(50x75)=20</t>
         </is>
@@ -1368,18 +1517,29 @@
           <t>#4</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr"/>
+      <c r="C5" s="4" t="n">
+        <v>50</v>
+      </c>
       <c r="D5" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="E5" s="4" t="n"/>
+      <c r="F5" s="4" t="n"/>
+      <c r="G5" s="4" t="n"/>
+      <c r="H5" s="4" t="n"/>
+      <c r="I5" s="4" t="n"/>
+      <c r="J5" s="5" t="inlineStr"/>
+      <c r="K5" s="4" t="n">
         <v>125</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="L5" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="M5" s="4" t="n">
         <v>124</v>
       </c>
-      <c r="G5" s="4" t="inlineStr"/>
-      <c r="H5" s="4" t="inlineStr">
+      <c r="N5" s="4" t="inlineStr"/>
+      <c r="O5" s="4" t="inlineStr">
         <is>
           <t>L箍#4(50+75)=20</t>
         </is>
@@ -1394,18 +1554,29 @@
           <t>#5</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr"/>
+      <c r="C6" s="4" t="n">
+        <v>50</v>
+      </c>
       <c r="D6" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="E6" s="4" t="n"/>
+      <c r="F6" s="4" t="n"/>
+      <c r="G6" s="4" t="n"/>
+      <c r="H6" s="4" t="n"/>
+      <c r="I6" s="4" t="n"/>
+      <c r="J6" s="5" t="inlineStr"/>
+      <c r="K6" s="4" t="n">
         <v>125</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="L6" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="M6" s="4" t="n">
         <v>194</v>
       </c>
-      <c r="G6" s="4" t="inlineStr"/>
-      <c r="H6" s="4" t="inlineStr">
+      <c r="N6" s="4" t="inlineStr"/>
+      <c r="O6" s="4" t="inlineStr">
         <is>
           <t>U箍#5(50x75)=20</t>
         </is>
@@ -1420,18 +1591,29 @@
           <t>#4</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr"/>
+      <c r="C7" s="4" t="n">
+        <v>50</v>
+      </c>
       <c r="D7" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="E7" s="4" t="n"/>
+      <c r="F7" s="4" t="n"/>
+      <c r="G7" s="4" t="n"/>
+      <c r="H7" s="4" t="n"/>
+      <c r="I7" s="4" t="n"/>
+      <c r="J7" s="5" t="inlineStr"/>
+      <c r="K7" s="4" t="n">
         <v>125</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="L7" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="M7" s="4" t="n">
         <v>124</v>
       </c>
-      <c r="G7" s="4" t="inlineStr"/>
-      <c r="H7" s="4" t="inlineStr">
+      <c r="N7" s="4" t="inlineStr"/>
+      <c r="O7" s="4" t="inlineStr">
         <is>
           <t>牆箍#4(50x75)=20</t>
         </is>
@@ -1446,18 +1628,29 @@
           <t>#4</t>
         </is>
       </c>
-      <c r="C8" s="5" t="inlineStr"/>
+      <c r="C8" s="4" t="n">
+        <v>50</v>
+      </c>
       <c r="D8" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="E8" s="4" t="n"/>
+      <c r="F8" s="4" t="n"/>
+      <c r="G8" s="4" t="n"/>
+      <c r="H8" s="4" t="n"/>
+      <c r="I8" s="4" t="n"/>
+      <c r="J8" s="5" t="inlineStr"/>
+      <c r="K8" s="4" t="n">
         <v>125</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="L8" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F8" s="4" t="n">
+      <c r="M8" s="4" t="n">
         <v>124</v>
       </c>
-      <c r="G8" s="4" t="inlineStr"/>
-      <c r="H8" s="4" t="inlineStr">
+      <c r="N8" s="4" t="inlineStr"/>
+      <c r="O8" s="4" t="inlineStr">
         <is>
           <t>柱箍#4(50x75)=20</t>
         </is>
@@ -1472,18 +1665,29 @@
           <t>#3</t>
         </is>
       </c>
-      <c r="C9" s="5" t="inlineStr"/>
+      <c r="C9" s="4" t="n">
+        <v>50</v>
+      </c>
       <c r="D9" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="E9" s="4" t="n"/>
+      <c r="F9" s="4" t="n"/>
+      <c r="G9" s="4" t="n"/>
+      <c r="H9" s="4" t="n"/>
+      <c r="I9" s="4" t="n"/>
+      <c r="J9" s="5" t="inlineStr"/>
+      <c r="K9" s="4" t="n">
         <v>125</v>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="L9" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="M9" s="4" t="n">
         <v>70</v>
       </c>
-      <c r="G9" s="4" t="inlineStr"/>
-      <c r="H9" s="4" t="inlineStr">
+      <c r="N9" s="4" t="inlineStr"/>
+      <c r="O9" s="4" t="inlineStr">
         <is>
           <t>半箍#3(50+75)=20</t>
         </is>
@@ -1541,17 +1745,17 @@
     <row r="14">
       <c r="A14" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-23 13:48:36 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-23 14:06:48 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H14"/>
+  <autoFilter ref="A2:O14"/>
   <mergeCells count="4">
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A11:O11"/>
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="A2:O2"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape"/>
@@ -1573,7 +1777,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -1583,13 +1787,20 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="60" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="45" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="9" max="9"/>
+    <col width="60" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="45" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -1619,30 +1830,65 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
+          <t>A(cm)</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>B(cm)</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>C(cm)</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>D(cm)</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>E(cm)</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>F(cm)</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>G(cm)</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
           <t>圖示</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="K3" s="3" t="inlineStr">
         <is>
           <t>長度(cm)</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="L3" s="3" t="inlineStr">
         <is>
           <t>數量</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="M3" s="3" t="inlineStr">
         <is>
           <t>重量(kg)</t>
         </is>
       </c>
-      <c r="G3" s="3" t="inlineStr">
+      <c r="N3" s="3" t="inlineStr">
         <is>
           <t>備註</t>
         </is>
       </c>
-      <c r="H3" s="3" t="inlineStr">
+      <c r="O3" s="3" t="inlineStr">
         <is>
           <t>讀取CAD文字</t>
         </is>
@@ -1657,22 +1903,31 @@
           <t>#5</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr"/>
-      <c r="D4" s="4" t="n">
+      <c r="C4" s="4" t="n">
         <v>3000</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="D4" s="4" t="n"/>
+      <c r="E4" s="4" t="n"/>
+      <c r="F4" s="4" t="n"/>
+      <c r="G4" s="4" t="n"/>
+      <c r="H4" s="4" t="n"/>
+      <c r="I4" s="4" t="n"/>
+      <c r="J4" s="5" t="inlineStr"/>
+      <c r="K4" s="4" t="n">
+        <v>3000</v>
+      </c>
+      <c r="L4" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="M4" s="4" t="n">
         <v>4656</v>
       </c>
-      <c r="G4" s="4" t="inlineStr">
+      <c r="N4" s="4" t="inlineStr">
         <is>
           <t>安</t>
         </is>
       </c>
-      <c r="H4" s="4" t="inlineStr">
+      <c r="O4" s="4" t="inlineStr">
         <is>
           <t>安#5-3000x20</t>
         </is>
@@ -1687,22 +1942,31 @@
           <t>#5</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr"/>
-      <c r="D5" s="4" t="n">
+      <c r="C5" s="4" t="n">
         <v>85</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="D5" s="4" t="n"/>
+      <c r="E5" s="4" t="n"/>
+      <c r="F5" s="4" t="n"/>
+      <c r="G5" s="4" t="n"/>
+      <c r="H5" s="4" t="n"/>
+      <c r="I5" s="4" t="n"/>
+      <c r="J5" s="5" t="inlineStr"/>
+      <c r="K5" s="4" t="n">
+        <v>85</v>
+      </c>
+      <c r="L5" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="M5" s="4" t="n">
         <v>132</v>
       </c>
-      <c r="G5" s="4" t="inlineStr">
+      <c r="N5" s="4" t="inlineStr">
         <is>
           <t>安</t>
         </is>
       </c>
-      <c r="H5" s="4" t="inlineStr">
+      <c r="O5" s="4" t="inlineStr">
         <is>
           <t>安#5-85x20</t>
         </is>
@@ -1717,22 +1981,33 @@
           <t>#5</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr"/>
+      <c r="C6" s="4" t="n">
+        <v>25</v>
+      </c>
       <c r="D6" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="4" t="n"/>
+      <c r="F6" s="4" t="n"/>
+      <c r="G6" s="4" t="n"/>
+      <c r="H6" s="4" t="n"/>
+      <c r="I6" s="4" t="n"/>
+      <c r="J6" s="5" t="inlineStr"/>
+      <c r="K6" s="4" t="n">
         <v>1025</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="L6" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="M6" s="4" t="n">
         <v>1591</v>
       </c>
-      <c r="G6" s="4" t="inlineStr">
+      <c r="N6" s="4" t="inlineStr">
         <is>
           <t>安</t>
         </is>
       </c>
-      <c r="H6" s="4" t="inlineStr">
+      <c r="O6" s="4" t="inlineStr">
         <is>
           <t>安#5-25+1000x20</t>
         </is>
@@ -1747,22 +2022,33 @@
           <t>#4</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr"/>
+      <c r="C7" s="4" t="n">
+        <v>30</v>
+      </c>
       <c r="D7" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="E7" s="4" t="n"/>
+      <c r="F7" s="4" t="n"/>
+      <c r="G7" s="4" t="n"/>
+      <c r="H7" s="4" t="n"/>
+      <c r="I7" s="4" t="n"/>
+      <c r="J7" s="5" t="inlineStr"/>
+      <c r="K7" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="L7" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="M7" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="G7" s="4" t="inlineStr">
+      <c r="N7" s="4" t="inlineStr">
         <is>
           <t>安</t>
         </is>
       </c>
-      <c r="H7" s="4" t="inlineStr">
+      <c r="O7" s="4" t="inlineStr">
         <is>
           <t>安#4-30+60x20</t>
         </is>
@@ -1820,17 +2106,17 @@
     <row r="12">
       <c r="A12" s="9" t="inlineStr">
         <is>
-          <t>生成時間：2025-06-23 13:48:36 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
+          <t>生成時間：2025-06-23 14:06:48 | 圖示模式：圖文混合模式 | 圖形功能：啟用</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H12"/>
+  <autoFilter ref="A2:O12"/>
   <mergeCells count="4">
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A9:O9"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A12:O12"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape"/>

</xml_diff>